<commit_message>
Update Streamlit page [2] & Data analysis
</commit_message>
<xml_diff>
--- a/Roadmap champignons.xlsx
+++ b/Roadmap champignons.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t xml:space="preserve">Cat</t>
   </si>
@@ -80,15 +80,36 @@
     <t xml:space="preserve">/src/notebooks/2-data_analysis.ipynb</t>
   </si>
   <si>
+    <t xml:space="preserve">Analyses images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyses des images (colorimétrie, dimensions)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/src/notebooks/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3-imgs_analysis.ipynb</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">En cours</t>
   </si>
   <si>
-    <t xml:space="preserve">Analyses images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analyses des images (colorimétrie, dimensions)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modèle 1 - Classification champi/not champi</t>
   </si>
   <si>
@@ -116,7 +137,10 @@
     <t xml:space="preserve">originaldatasetpage.py</t>
   </si>
   <si>
-    <t xml:space="preserve">Page Data Visualisation</t>
+    <t xml:space="preserve">Page Data Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataanalysispage.py</t>
   </si>
   <si>
     <t xml:space="preserve">654</t>
@@ -144,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -194,6 +218,12 @@
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -393,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -494,11 +524,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -602,7 +632,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -675,10 +705,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,11 +744,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,12 +914,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,25 +1028,29 @@
         <v>18</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="D8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
+      <c r="E8" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="27"/>
     </row>
     <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
@@ -1063,7 +1093,7 @@
     <row r="14" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="28"/>
       <c r="B14" s="33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="34"/>
@@ -1088,7 +1118,7 @@
     </row>
     <row r="17" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
@@ -1155,7 +1185,7 @@
     <row r="25" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="41"/>
       <c r="B25" s="45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" s="45"/>
       <c r="D25" s="46"/>
@@ -1172,7 +1202,7 @@
     </row>
     <row r="27" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="53" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="54"/>
       <c r="C27" s="54"/>
@@ -1239,7 +1269,7 @@
     <row r="35" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="53"/>
       <c r="B35" s="61" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C35" s="61"/>
       <c r="D35" s="62"/>
@@ -1256,17 +1286,17 @@
     </row>
     <row r="37" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" s="67"/>
       <c r="C37" s="67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D37" s="68" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E37" s="68" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F37" s="69"/>
     </row>
@@ -1274,13 +1304,13 @@
       <c r="A38" s="19"/>
       <c r="B38" s="70"/>
       <c r="C38" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="71" t="s">
         <v>30</v>
       </c>
+      <c r="D38" s="26" t="s">
+        <v>31</v>
+      </c>
       <c r="E38" s="26" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F38" s="27"/>
     </row>
@@ -1288,84 +1318,120 @@
       <c r="A39" s="19"/>
       <c r="B39" s="70"/>
       <c r="C39" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="71"/>
-      <c r="E39" s="26"/>
+        <v>32</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="F39" s="27"/>
     </row>
     <row r="40" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="19"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="74"/>
-    </row>
-    <row r="41" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="75"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-    </row>
-    <row r="42" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="77"/>
-      <c r="B42" s="78"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-    </row>
-    <row r="43" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="77"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-    </row>
-    <row r="44" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="77"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="19"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="27"/>
+    </row>
+    <row r="42" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="19"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="27"/>
+    </row>
+    <row r="43" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="19"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="27"/>
+    </row>
+    <row r="44" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="19"/>
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="73"/>
     </row>
     <row r="45" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="77"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
+      <c r="A45" s="74"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
     </row>
     <row r="46" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="77"/>
-      <c r="B46" s="78"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="78"/>
-      <c r="F46" s="78"/>
+      <c r="A46" s="76"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="77"/>
     </row>
     <row r="47" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="77"/>
-      <c r="B47" s="78"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-    </row>
-    <row r="48" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A47" s="76"/>
+      <c r="B47" s="77"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="77"/>
+    </row>
+    <row r="48" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="76"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
+    </row>
+    <row r="49" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="76"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="77"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="77"/>
+    </row>
+    <row r="50" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="76"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="77"/>
+      <c r="D50" s="77"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="77"/>
+    </row>
+    <row r="51" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="76"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="77"/>
+    </row>
     <row r="52" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:A6"/>
@@ -1375,7 +1441,7 @@
     <mergeCell ref="A9:A16"/>
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="A27:A36"/>
-    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A37:A44"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -1441,363 +1507,363 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="B1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="C1" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="D1" s="79" t="s">
         <v>37</v>
       </c>
+      <c r="E1" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="81"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
     </row>
     <row r="3" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="81"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
+      <c r="A3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
     </row>
     <row r="4" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="81"/>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="52"/>
-      <c r="F4" s="82"/>
+      <c r="F4" s="81"/>
     </row>
     <row r="5" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="81"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
     </row>
     <row r="6" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="81"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
     </row>
     <row r="7" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="81"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
       <c r="E7" s="52"/>
-      <c r="F7" s="82"/>
+      <c r="F7" s="81"/>
     </row>
     <row r="8" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="81"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
       <c r="F8" s="52"/>
     </row>
     <row r="9" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="81"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
       <c r="F9" s="52"/>
     </row>
     <row r="10" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="81"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
       <c r="F10" s="52"/>
     </row>
     <row r="11" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="81"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="52"/>
     </row>
     <row r="12" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="81"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="81"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
       <c r="F13" s="52"/>
     </row>
     <row r="14" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="81"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
       <c r="F14" s="52"/>
     </row>
     <row r="15" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="81"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
       <c r="F15" s="52"/>
     </row>
     <row r="16" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="81"/>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="52"/>
-      <c r="F16" s="82"/>
+      <c r="F16" s="81"/>
     </row>
     <row r="17" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="81"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="52"/>
-      <c r="F17" s="82"/>
+      <c r="F17" s="81"/>
     </row>
     <row r="18" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="81"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="52"/>
-      <c r="F18" s="82"/>
+      <c r="F18" s="81"/>
     </row>
     <row r="19" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="81"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="52"/>
-      <c r="F19" s="82"/>
+      <c r="F19" s="81"/>
     </row>
     <row r="20" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="81"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
+      <c r="A20" s="80"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
       <c r="E20" s="52"/>
-      <c r="F20" s="82"/>
+      <c r="F20" s="81"/>
     </row>
     <row r="21" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="81"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
       <c r="E21" s="52"/>
-      <c r="F21" s="82"/>
+      <c r="F21" s="81"/>
     </row>
     <row r="22" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="81"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
       <c r="E22" s="52"/>
-      <c r="F22" s="82"/>
+      <c r="F22" s="81"/>
     </row>
     <row r="23" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="81"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="82"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="52"/>
-      <c r="F23" s="82"/>
+      <c r="F23" s="81"/>
     </row>
     <row r="24" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="81"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
-      <c r="D24" s="82"/>
+      <c r="D24" s="81"/>
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
     </row>
     <row r="25" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="81"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
     </row>
     <row r="26" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="81"/>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
     </row>
     <row r="27" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="81"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
     </row>
     <row r="28" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="81"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
     </row>
     <row r="29" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="81"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="82"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
     </row>
     <row r="30" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="81"/>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
+      <c r="A30" s="80"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
     </row>
     <row r="31" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="81"/>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
       <c r="F31" s="52"/>
     </row>
     <row r="32" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="81"/>
+      <c r="A32" s="80"/>
       <c r="B32" s="52"/>
       <c r="C32" s="52"/>
-      <c r="D32" s="82"/>
+      <c r="D32" s="81"/>
       <c r="E32" s="52"/>
       <c r="F32" s="52"/>
     </row>
     <row r="33" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="81"/>
+      <c r="A33" s="80"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
-      <c r="D33" s="82"/>
+      <c r="D33" s="81"/>
       <c r="E33" s="52"/>
       <c r="F33" s="52"/>
     </row>
     <row r="34" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="81"/>
+      <c r="A34" s="80"/>
       <c r="B34" s="52"/>
       <c r="C34" s="52"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
       <c r="F34" s="52"/>
     </row>
     <row r="35" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="81"/>
+      <c r="A35" s="80"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
       <c r="F35" s="52"/>
     </row>
     <row r="36" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="81"/>
+      <c r="A36" s="80"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
       <c r="F36" s="52"/>
     </row>
     <row r="37" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="81"/>
+      <c r="A37" s="80"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
       <c r="F37" s="52"/>
     </row>
     <row r="38" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="81"/>
+      <c r="A38" s="80"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
       <c r="F38" s="52"/>
     </row>
     <row r="39" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="81"/>
+      <c r="A39" s="80"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
       <c r="F39" s="52"/>
     </row>
     <row r="40" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="81"/>
+      <c r="A40" s="80"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
       <c r="F40" s="52"/>
     </row>
     <row r="41" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="81"/>
+      <c r="A41" s="80"/>
       <c r="B41" s="52"/>
       <c r="C41" s="52"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
       <c r="F41" s="52"/>
     </row>
     <row r="42" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="81"/>
+      <c r="A42" s="80"/>
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
       <c r="F42" s="52"/>
     </row>
     <row r="43" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="81"/>
+      <c r="A43" s="80"/>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>
-      <c r="D43" s="82"/>
+      <c r="D43" s="81"/>
       <c r="E43" s="52"/>
       <c r="F43" s="52"/>
     </row>
     <row r="44" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="81"/>
+      <c r="A44" s="80"/>
       <c r="B44" s="52"/>
       <c r="C44" s="52"/>
       <c r="D44" s="52"/>
@@ -1805,7 +1871,7 @@
       <c r="F44" s="52"/>
     </row>
     <row r="45" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="81"/>
+      <c r="A45" s="80"/>
       <c r="B45" s="52"/>
       <c r="C45" s="52"/>
       <c r="D45" s="52"/>
@@ -1813,7 +1879,7 @@
       <c r="F45" s="52"/>
     </row>
     <row r="46" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="81"/>
+      <c r="A46" s="80"/>
       <c r="B46" s="52"/>
       <c r="C46" s="52"/>
       <c r="D46" s="52"/>
@@ -1821,7 +1887,7 @@
       <c r="F46" s="52"/>
     </row>
     <row r="47" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="81"/>
+      <c r="A47" s="80"/>
       <c r="B47" s="52"/>
       <c r="C47" s="52"/>
       <c r="D47" s="52"/>
@@ -1829,7 +1895,7 @@
       <c r="F47" s="52"/>
     </row>
     <row r="48" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="81"/>
+      <c r="A48" s="80"/>
       <c r="B48" s="52"/>
       <c r="C48" s="52"/>
       <c r="D48" s="52"/>
@@ -1837,332 +1903,332 @@
       <c r="F48" s="52"/>
     </row>
     <row r="49" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="81"/>
+      <c r="A49" s="80"/>
       <c r="B49" s="52"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
     </row>
     <row r="50" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="81"/>
+      <c r="A50" s="80"/>
       <c r="B50" s="52"/>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
     </row>
     <row r="51" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="81"/>
+      <c r="A51" s="80"/>
       <c r="B51" s="52"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="81"/>
     </row>
     <row r="52" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="81"/>
+      <c r="A52" s="80"/>
       <c r="B52" s="52"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="81"/>
     </row>
     <row r="53" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="81"/>
+      <c r="A53" s="80"/>
       <c r="B53" s="52"/>
-      <c r="C53" s="82"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="81"/>
     </row>
     <row r="54" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="81"/>
+      <c r="A54" s="80"/>
       <c r="B54" s="52"/>
-      <c r="C54" s="82"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="82"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
       <c r="F54" s="52"/>
     </row>
     <row r="55" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="81"/>
-      <c r="B55" s="82"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="82"/>
+      <c r="A55" s="80"/>
+      <c r="B55" s="81"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
       <c r="E55" s="52"/>
-      <c r="F55" s="82"/>
+      <c r="F55" s="81"/>
     </row>
     <row r="56" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="81"/>
-      <c r="B56" s="82"/>
-      <c r="C56" s="82"/>
-      <c r="D56" s="82"/>
+      <c r="A56" s="80"/>
+      <c r="B56" s="81"/>
+      <c r="C56" s="81"/>
+      <c r="D56" s="81"/>
       <c r="E56" s="52"/>
-      <c r="F56" s="82"/>
+      <c r="F56" s="81"/>
     </row>
     <row r="57" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="81"/>
-      <c r="B57" s="82"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="82"/>
+      <c r="A57" s="80"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="81"/>
+      <c r="D57" s="81"/>
       <c r="E57" s="52"/>
-      <c r="F57" s="82"/>
+      <c r="F57" s="81"/>
     </row>
     <row r="58" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="81"/>
-      <c r="B58" s="82"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="82"/>
+      <c r="A58" s="80"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="81"/>
+      <c r="D58" s="81"/>
       <c r="E58" s="52"/>
-      <c r="F58" s="82"/>
+      <c r="F58" s="81"/>
     </row>
     <row r="59" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="81"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="82"/>
-      <c r="D59" s="82"/>
+      <c r="A59" s="80"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="81"/>
+      <c r="D59" s="81"/>
       <c r="E59" s="52"/>
-      <c r="F59" s="82"/>
+      <c r="F59" s="81"/>
     </row>
     <row r="60" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="81"/>
-      <c r="B60" s="82"/>
-      <c r="C60" s="82"/>
-      <c r="D60" s="82"/>
+      <c r="A60" s="80"/>
+      <c r="B60" s="81"/>
+      <c r="C60" s="81"/>
+      <c r="D60" s="81"/>
       <c r="E60" s="52"/>
-      <c r="F60" s="82"/>
+      <c r="F60" s="81"/>
     </row>
     <row r="61" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="81"/>
-      <c r="B61" s="82"/>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
+      <c r="A61" s="80"/>
+      <c r="B61" s="81"/>
+      <c r="C61" s="81"/>
+      <c r="D61" s="81"/>
       <c r="E61" s="52"/>
-      <c r="F61" s="82"/>
+      <c r="F61" s="81"/>
     </row>
     <row r="62" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="81"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="82"/>
-      <c r="D62" s="82"/>
+      <c r="A62" s="80"/>
+      <c r="B62" s="81"/>
+      <c r="C62" s="81"/>
+      <c r="D62" s="81"/>
       <c r="E62" s="52"/>
-      <c r="F62" s="82"/>
+      <c r="F62" s="81"/>
     </row>
     <row r="63" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="81"/>
-      <c r="B63" s="82"/>
-      <c r="C63" s="82"/>
-      <c r="D63" s="82"/>
+      <c r="A63" s="80"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="81"/>
+      <c r="D63" s="81"/>
       <c r="E63" s="52"/>
-      <c r="F63" s="82"/>
+      <c r="F63" s="81"/>
     </row>
     <row r="64" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="81"/>
-      <c r="B64" s="82"/>
-      <c r="C64" s="82"/>
-      <c r="D64" s="82"/>
+      <c r="A64" s="80"/>
+      <c r="B64" s="81"/>
+      <c r="C64" s="81"/>
+      <c r="D64" s="81"/>
       <c r="E64" s="52"/>
-      <c r="F64" s="82"/>
+      <c r="F64" s="81"/>
     </row>
     <row r="65" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="81"/>
-      <c r="B65" s="82"/>
-      <c r="C65" s="82"/>
-      <c r="D65" s="82"/>
+      <c r="A65" s="80"/>
+      <c r="B65" s="81"/>
+      <c r="C65" s="81"/>
+      <c r="D65" s="81"/>
       <c r="E65" s="52"/>
-      <c r="F65" s="82"/>
+      <c r="F65" s="81"/>
     </row>
     <row r="66" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="81"/>
-      <c r="B66" s="82"/>
-      <c r="C66" s="82"/>
-      <c r="D66" s="82"/>
+      <c r="A66" s="80"/>
+      <c r="B66" s="81"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="81"/>
       <c r="E66" s="52"/>
-      <c r="F66" s="82"/>
+      <c r="F66" s="81"/>
     </row>
     <row r="67" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="81"/>
-      <c r="B67" s="82"/>
-      <c r="C67" s="82"/>
-      <c r="D67" s="82"/>
+      <c r="A67" s="80"/>
+      <c r="B67" s="81"/>
+      <c r="C67" s="81"/>
+      <c r="D67" s="81"/>
       <c r="E67" s="52"/>
-      <c r="F67" s="82"/>
+      <c r="F67" s="81"/>
     </row>
     <row r="68" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="81"/>
-      <c r="B68" s="82"/>
-      <c r="C68" s="82"/>
-      <c r="D68" s="82"/>
+      <c r="A68" s="80"/>
+      <c r="B68" s="81"/>
+      <c r="C68" s="81"/>
+      <c r="D68" s="81"/>
       <c r="E68" s="52"/>
-      <c r="F68" s="82"/>
+      <c r="F68" s="81"/>
     </row>
     <row r="69" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="81"/>
-      <c r="B69" s="82"/>
-      <c r="C69" s="82"/>
-      <c r="D69" s="82"/>
+      <c r="A69" s="80"/>
+      <c r="B69" s="81"/>
+      <c r="C69" s="81"/>
+      <c r="D69" s="81"/>
       <c r="E69" s="52"/>
-      <c r="F69" s="82"/>
+      <c r="F69" s="81"/>
     </row>
     <row r="70" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="81"/>
-      <c r="B70" s="82"/>
-      <c r="C70" s="82"/>
-      <c r="D70" s="82"/>
+      <c r="A70" s="80"/>
+      <c r="B70" s="81"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="81"/>
       <c r="E70" s="52"/>
-      <c r="F70" s="82"/>
+      <c r="F70" s="81"/>
     </row>
     <row r="71" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="81"/>
-      <c r="B71" s="82"/>
-      <c r="C71" s="82"/>
-      <c r="D71" s="82"/>
+      <c r="A71" s="80"/>
+      <c r="B71" s="81"/>
+      <c r="C71" s="81"/>
+      <c r="D71" s="81"/>
       <c r="E71" s="52"/>
-      <c r="F71" s="82"/>
+      <c r="F71" s="81"/>
     </row>
     <row r="72" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="81"/>
-      <c r="B72" s="82"/>
-      <c r="C72" s="82"/>
-      <c r="D72" s="82"/>
+      <c r="A72" s="80"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="81"/>
+      <c r="D72" s="81"/>
       <c r="E72" s="52"/>
-      <c r="F72" s="82"/>
+      <c r="F72" s="81"/>
     </row>
     <row r="73" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="81"/>
-      <c r="B73" s="82"/>
-      <c r="C73" s="82"/>
-      <c r="D73" s="82"/>
+      <c r="A73" s="80"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="81"/>
+      <c r="D73" s="81"/>
       <c r="E73" s="52"/>
-      <c r="F73" s="82"/>
+      <c r="F73" s="81"/>
     </row>
     <row r="74" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="81"/>
-      <c r="B74" s="82"/>
-      <c r="C74" s="82"/>
-      <c r="D74" s="82"/>
+      <c r="A74" s="80"/>
+      <c r="B74" s="81"/>
+      <c r="C74" s="81"/>
+      <c r="D74" s="81"/>
       <c r="E74" s="52"/>
-      <c r="F74" s="82"/>
+      <c r="F74" s="81"/>
     </row>
     <row r="75" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="81"/>
-      <c r="B75" s="82"/>
-      <c r="C75" s="82"/>
-      <c r="D75" s="82"/>
+      <c r="A75" s="80"/>
+      <c r="B75" s="81"/>
+      <c r="C75" s="81"/>
+      <c r="D75" s="81"/>
       <c r="E75" s="52"/>
-      <c r="F75" s="82"/>
+      <c r="F75" s="81"/>
     </row>
     <row r="76" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="81"/>
-      <c r="B76" s="82"/>
-      <c r="C76" s="82"/>
-      <c r="D76" s="82"/>
+      <c r="A76" s="80"/>
+      <c r="B76" s="81"/>
+      <c r="C76" s="81"/>
+      <c r="D76" s="81"/>
       <c r="E76" s="52"/>
-      <c r="F76" s="82"/>
+      <c r="F76" s="81"/>
     </row>
     <row r="77" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="81"/>
-      <c r="B77" s="82"/>
-      <c r="C77" s="82"/>
-      <c r="D77" s="82"/>
+      <c r="A77" s="80"/>
+      <c r="B77" s="81"/>
+      <c r="C77" s="81"/>
+      <c r="D77" s="81"/>
       <c r="E77" s="52"/>
-      <c r="F77" s="82"/>
+      <c r="F77" s="81"/>
     </row>
     <row r="78" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="81"/>
-      <c r="B78" s="82"/>
-      <c r="C78" s="82"/>
-      <c r="D78" s="82"/>
+      <c r="A78" s="80"/>
+      <c r="B78" s="81"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="81"/>
       <c r="E78" s="52"/>
-      <c r="F78" s="82"/>
+      <c r="F78" s="81"/>
     </row>
     <row r="79" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="81"/>
-      <c r="B79" s="82"/>
-      <c r="C79" s="82"/>
-      <c r="D79" s="82"/>
+      <c r="A79" s="80"/>
+      <c r="B79" s="81"/>
+      <c r="C79" s="81"/>
+      <c r="D79" s="81"/>
       <c r="E79" s="52"/>
-      <c r="F79" s="82"/>
+      <c r="F79" s="81"/>
     </row>
     <row r="80" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="81"/>
-      <c r="B80" s="82"/>
-      <c r="C80" s="82"/>
-      <c r="D80" s="82"/>
+      <c r="A80" s="80"/>
+      <c r="B80" s="81"/>
+      <c r="C80" s="81"/>
+      <c r="D80" s="81"/>
       <c r="E80" s="52"/>
-      <c r="F80" s="82"/>
+      <c r="F80" s="81"/>
     </row>
     <row r="81" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="81"/>
-      <c r="B81" s="82"/>
-      <c r="C81" s="82"/>
-      <c r="D81" s="82"/>
+      <c r="A81" s="80"/>
+      <c r="B81" s="81"/>
+      <c r="C81" s="81"/>
+      <c r="D81" s="81"/>
       <c r="E81" s="52"/>
-      <c r="F81" s="82"/>
+      <c r="F81" s="81"/>
     </row>
     <row r="82" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="81"/>
-      <c r="B82" s="82"/>
-      <c r="C82" s="82"/>
-      <c r="D82" s="82"/>
+      <c r="A82" s="80"/>
+      <c r="B82" s="81"/>
+      <c r="C82" s="81"/>
+      <c r="D82" s="81"/>
       <c r="E82" s="52"/>
-      <c r="F82" s="82"/>
+      <c r="F82" s="81"/>
     </row>
     <row r="83" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="81"/>
-      <c r="B83" s="82"/>
-      <c r="C83" s="82"/>
-      <c r="D83" s="82"/>
+      <c r="A83" s="80"/>
+      <c r="B83" s="81"/>
+      <c r="C83" s="81"/>
+      <c r="D83" s="81"/>
       <c r="E83" s="52"/>
-      <c r="F83" s="82"/>
+      <c r="F83" s="81"/>
     </row>
     <row r="84" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="81"/>
-      <c r="B84" s="82"/>
-      <c r="C84" s="82"/>
-      <c r="D84" s="82"/>
+      <c r="A84" s="80"/>
+      <c r="B84" s="81"/>
+      <c r="C84" s="81"/>
+      <c r="D84" s="81"/>
       <c r="E84" s="52"/>
-      <c r="F84" s="82"/>
+      <c r="F84" s="81"/>
     </row>
     <row r="85" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="81"/>
-      <c r="B85" s="82"/>
-      <c r="C85" s="82"/>
-      <c r="D85" s="82"/>
+      <c r="A85" s="80"/>
+      <c r="B85" s="81"/>
+      <c r="C85" s="81"/>
+      <c r="D85" s="81"/>
       <c r="E85" s="52"/>
-      <c r="F85" s="82"/>
+      <c r="F85" s="81"/>
     </row>
     <row r="86" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="81"/>
-      <c r="B86" s="82"/>
-      <c r="C86" s="82"/>
-      <c r="D86" s="82"/>
+      <c r="A86" s="80"/>
+      <c r="B86" s="81"/>
+      <c r="C86" s="81"/>
+      <c r="D86" s="81"/>
       <c r="E86" s="52"/>
-      <c r="F86" s="82"/>
+      <c r="F86" s="81"/>
     </row>
     <row r="87" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="81"/>
-      <c r="B87" s="82"/>
-      <c r="C87" s="82"/>
-      <c r="D87" s="82"/>
+      <c r="A87" s="80"/>
+      <c r="B87" s="81"/>
+      <c r="C87" s="81"/>
+      <c r="D87" s="81"/>
       <c r="E87" s="52"/>
-      <c r="F87" s="82"/>
+      <c r="F87" s="81"/>
     </row>
     <row r="88" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="81"/>
-      <c r="B88" s="82"/>
-      <c r="C88" s="82"/>
-      <c r="D88" s="82"/>
+      <c r="A88" s="80"/>
+      <c r="B88" s="81"/>
+      <c r="C88" s="81"/>
+      <c r="D88" s="81"/>
       <c r="E88" s="52"/>
-      <c r="F88" s="82"/>
+      <c r="F88" s="81"/>
     </row>
     <row r="89" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="81"/>
-      <c r="B89" s="82"/>
-      <c r="C89" s="82"/>
-      <c r="D89" s="82"/>
+      <c r="A89" s="80"/>
+      <c r="B89" s="81"/>
+      <c r="C89" s="81"/>
+      <c r="D89" s="81"/>
       <c r="E89" s="52"/>
-      <c r="F89" s="82"/>
+      <c r="F89" s="81"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update img analysis, starting img preprocessing
</commit_message>
<xml_diff>
--- a/Roadmap champignons.xlsx
+++ b/Roadmap champignons.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t xml:space="preserve">Cat</t>
   </si>
@@ -66,6 +66,36 @@
   </si>
   <si>
     <t xml:space="preserve">Script .py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification Choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choix classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/src/notebooks/4-classification_choice.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tri images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tri images (script) selon choix classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tri images manuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrait des images de mauvaise qualité « à la main »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAJ CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise à jour données CSV suite tri images</t>
   </si>
   <si>
     <t xml:space="preserve">Analyses</t>
@@ -92,6 +122,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/src/notebooks/</t>
     </r>
@@ -107,19 +138,22 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">En cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modèle 1 - Classification champi/not champi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mlflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modèle 2 - Cadrage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modèle 3 - Classification espèce</t>
+    <t xml:space="preserve">Image Pre-processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preprocessing images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Générer DataFrame Features &amp; Targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charger, transformer les images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Générer les datasets Tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modèle 1 – Specy Classification</t>
   </si>
   <si>
     <t xml:space="preserve">Streamlit</t>
@@ -141,6 +175,24 @@
   </si>
   <si>
     <t xml:space="preserve">dataanalysispage.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Classification Choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classificationchoicepage.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Data preprocessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Modelization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model 1 ; Model 2 (modelization, training, evaluation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Prediction</t>
   </si>
   <si>
     <t xml:space="preserve">654</t>
@@ -168,7 +220,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -221,6 +273,18 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -472,15 +536,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,11 +564,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,7 +596,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -548,7 +620,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,14 +636,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -588,7 +664,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -616,10 +692,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -632,7 +704,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,22 +724,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -712,7 +768,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,11 +808,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,17 +978,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="77.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="55.72"/>
@@ -992,142 +1056,184 @@
     </row>
     <row r="4" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+      <c r="B5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="22" t="s">
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
-      <c r="B8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21"/>
+      <c r="B9" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="27"/>
-    </row>
-    <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
-    </row>
-    <row r="10" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="28"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="36"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28"/>
-      <c r="B14" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41"/>
+      <c r="A18" s="44" t="s">
+        <v>37</v>
+      </c>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
       <c r="D18" s="46"/>
@@ -1135,313 +1241,229 @@
       <c r="F18" s="47"/>
     </row>
     <row r="19" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
-    </row>
-    <row r="20" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+    </row>
+    <row r="20" s="54" customFormat="true" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="44"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="53"/>
     </row>
     <row r="21" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="47"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
     </row>
     <row r="22" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="61"/>
     </row>
     <row r="23" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="48"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
     </row>
     <row r="24" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47"/>
+      <c r="A24" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="67"/>
     </row>
     <row r="25" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41"/>
-      <c r="B25" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="47"/>
-    </row>
-    <row r="26" s="52" customFormat="true" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="56"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="53"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="59"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="53"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="60"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="53"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="59"/>
-    </row>
-    <row r="31" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="53"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="59"/>
-    </row>
-    <row r="32" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="53"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="63"/>
-    </row>
-    <row r="33" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="53"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="63"/>
-    </row>
-    <row r="34" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="53"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="63"/>
-    </row>
-    <row r="35" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="53"/>
-      <c r="B35" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="63"/>
-    </row>
-    <row r="36" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="53"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="66"/>
-    </row>
-    <row r="37" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="69"/>
-    </row>
-    <row r="38" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="19"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F38" s="27"/>
-    </row>
-    <row r="39" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" s="27"/>
-    </row>
-    <row r="40" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="19"/>
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="27"/>
-    </row>
-    <row r="41" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="27"/>
-    </row>
-    <row r="42" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="19"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="27"/>
-    </row>
-    <row r="43" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="19"/>
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="27"/>
-    </row>
-    <row r="44" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="19"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="73"/>
-    </row>
-    <row r="45" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="74"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-    </row>
-    <row r="46" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="76"/>
-      <c r="B46" s="77"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="77"/>
-    </row>
-    <row r="47" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="76"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-    </row>
-    <row r="48" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="76"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-    </row>
-    <row r="49" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="76"/>
-      <c r="B49" s="77"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="77"/>
-    </row>
-    <row r="50" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="76"/>
-      <c r="B50" s="77"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="77"/>
-      <c r="F50" s="77"/>
-    </row>
-    <row r="51" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="76"/>
-      <c r="B51" s="77"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-    </row>
-    <row r="52" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="71"/>
+      <c r="E30" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="73"/>
+    </row>
+    <row r="31" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="74"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+    </row>
+    <row r="32" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="76"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+    </row>
+    <row r="33" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="76"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+    </row>
+    <row r="34" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="76"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+    </row>
+    <row r="35" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="76"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+    </row>
+    <row r="36" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="76"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+    </row>
+    <row r="37" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="76"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+    </row>
+    <row r="38" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A30"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -1508,22 +1530,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="78" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D1" s="79" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E1" s="79" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F1" s="79" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1547,7 +1569,7 @@
       <c r="B4" s="81"/>
       <c r="C4" s="81"/>
       <c r="D4" s="81"/>
-      <c r="E4" s="52"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="81"/>
     </row>
     <row r="5" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1571,7 +1593,7 @@
       <c r="B7" s="81"/>
       <c r="C7" s="81"/>
       <c r="D7" s="81"/>
-      <c r="E7" s="52"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="81"/>
     </row>
     <row r="8" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1580,7 +1602,7 @@
       <c r="C8" s="81"/>
       <c r="D8" s="81"/>
       <c r="E8" s="81"/>
-      <c r="F8" s="52"/>
+      <c r="F8" s="54"/>
     </row>
     <row r="9" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="80"/>
@@ -1588,7 +1610,7 @@
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
       <c r="E9" s="81"/>
-      <c r="F9" s="52"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="80"/>
@@ -1596,7 +1618,7 @@
       <c r="C10" s="81"/>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
-      <c r="F10" s="52"/>
+      <c r="F10" s="54"/>
     </row>
     <row r="11" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="80"/>
@@ -1604,7 +1626,7 @@
       <c r="C11" s="81"/>
       <c r="D11" s="81"/>
       <c r="E11" s="81"/>
-      <c r="F11" s="52"/>
+      <c r="F11" s="54"/>
     </row>
     <row r="12" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="80"/>
@@ -1612,7 +1634,7 @@
       <c r="C12" s="81"/>
       <c r="D12" s="81"/>
       <c r="E12" s="81"/>
-      <c r="F12" s="52"/>
+      <c r="F12" s="54"/>
     </row>
     <row r="13" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="80"/>
@@ -1620,7 +1642,7 @@
       <c r="C13" s="81"/>
       <c r="D13" s="81"/>
       <c r="E13" s="81"/>
-      <c r="F13" s="52"/>
+      <c r="F13" s="54"/>
     </row>
     <row r="14" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="80"/>
@@ -1628,7 +1650,7 @@
       <c r="C14" s="81"/>
       <c r="D14" s="81"/>
       <c r="E14" s="81"/>
-      <c r="F14" s="52"/>
+      <c r="F14" s="54"/>
     </row>
     <row r="15" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="80"/>
@@ -1636,14 +1658,14 @@
       <c r="C15" s="81"/>
       <c r="D15" s="81"/>
       <c r="E15" s="81"/>
-      <c r="F15" s="52"/>
+      <c r="F15" s="54"/>
     </row>
     <row r="16" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="80"/>
       <c r="B16" s="81"/>
       <c r="C16" s="81"/>
       <c r="D16" s="81"/>
-      <c r="E16" s="52"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="81"/>
     </row>
     <row r="17" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1651,7 +1673,7 @@
       <c r="B17" s="81"/>
       <c r="C17" s="81"/>
       <c r="D17" s="81"/>
-      <c r="E17" s="52"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="81"/>
     </row>
     <row r="18" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1659,7 +1681,7 @@
       <c r="B18" s="81"/>
       <c r="C18" s="81"/>
       <c r="D18" s="81"/>
-      <c r="E18" s="52"/>
+      <c r="E18" s="54"/>
       <c r="F18" s="81"/>
     </row>
     <row r="19" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1667,7 +1689,7 @@
       <c r="B19" s="81"/>
       <c r="C19" s="81"/>
       <c r="D19" s="81"/>
-      <c r="E19" s="52"/>
+      <c r="E19" s="54"/>
       <c r="F19" s="81"/>
     </row>
     <row r="20" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1675,7 +1697,7 @@
       <c r="B20" s="81"/>
       <c r="C20" s="81"/>
       <c r="D20" s="81"/>
-      <c r="E20" s="52"/>
+      <c r="E20" s="54"/>
       <c r="F20" s="81"/>
     </row>
     <row r="21" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1683,7 +1705,7 @@
       <c r="B21" s="81"/>
       <c r="C21" s="81"/>
       <c r="D21" s="81"/>
-      <c r="E21" s="52"/>
+      <c r="E21" s="54"/>
       <c r="F21" s="81"/>
     </row>
     <row r="22" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1691,7 +1713,7 @@
       <c r="B22" s="81"/>
       <c r="C22" s="81"/>
       <c r="D22" s="81"/>
-      <c r="E22" s="52"/>
+      <c r="E22" s="54"/>
       <c r="F22" s="81"/>
     </row>
     <row r="23" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1699,16 +1721,16 @@
       <c r="B23" s="81"/>
       <c r="C23" s="81"/>
       <c r="D23" s="81"/>
-      <c r="E23" s="52"/>
+      <c r="E23" s="54"/>
       <c r="F23" s="81"/>
     </row>
     <row r="24" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="80"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
       <c r="D24" s="81"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
     </row>
     <row r="25" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="80"/>
@@ -1764,147 +1786,147 @@
       <c r="C31" s="81"/>
       <c r="D31" s="81"/>
       <c r="E31" s="81"/>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
     </row>
     <row r="32" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="80"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
       <c r="D32" s="81"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
     </row>
     <row r="33" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="80"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="81"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
     </row>
     <row r="34" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="80"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="81"/>
       <c r="E34" s="81"/>
-      <c r="F34" s="52"/>
+      <c r="F34" s="54"/>
     </row>
     <row r="35" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="80"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="81"/>
       <c r="E35" s="81"/>
-      <c r="F35" s="52"/>
+      <c r="F35" s="54"/>
     </row>
     <row r="36" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="80"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="81"/>
       <c r="E36" s="81"/>
-      <c r="F36" s="52"/>
+      <c r="F36" s="54"/>
     </row>
     <row r="37" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="80"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="81"/>
       <c r="E37" s="81"/>
-      <c r="F37" s="52"/>
+      <c r="F37" s="54"/>
     </row>
     <row r="38" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="80"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
       <c r="D38" s="81"/>
       <c r="E38" s="81"/>
-      <c r="F38" s="52"/>
+      <c r="F38" s="54"/>
     </row>
     <row r="39" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="80"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
       <c r="D39" s="81"/>
       <c r="E39" s="81"/>
-      <c r="F39" s="52"/>
+      <c r="F39" s="54"/>
     </row>
     <row r="40" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="80"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
       <c r="D40" s="81"/>
       <c r="E40" s="81"/>
-      <c r="F40" s="52"/>
+      <c r="F40" s="54"/>
     </row>
     <row r="41" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="80"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="52"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
       <c r="D41" s="81"/>
       <c r="E41" s="81"/>
-      <c r="F41" s="52"/>
+      <c r="F41" s="54"/>
     </row>
     <row r="42" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="80"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
       <c r="D42" s="81"/>
       <c r="E42" s="81"/>
-      <c r="F42" s="52"/>
+      <c r="F42" s="54"/>
     </row>
     <row r="43" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="80"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="52"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
       <c r="D43" s="81"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="52"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
     </row>
     <row r="44" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="80"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
     </row>
     <row r="45" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="80"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
     </row>
     <row r="46" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="80"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
     </row>
     <row r="47" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="80"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="52"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
     </row>
     <row r="48" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="80"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
     </row>
     <row r="49" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="80"/>
-      <c r="B49" s="52"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="81"/>
       <c r="D49" s="81"/>
       <c r="E49" s="81"/>
@@ -1912,7 +1934,7 @@
     </row>
     <row r="50" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="80"/>
-      <c r="B50" s="52"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="81"/>
       <c r="D50" s="81"/>
       <c r="E50" s="81"/>
@@ -1920,7 +1942,7 @@
     </row>
     <row r="51" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="80"/>
-      <c r="B51" s="52"/>
+      <c r="B51" s="54"/>
       <c r="C51" s="81"/>
       <c r="D51" s="81"/>
       <c r="E51" s="81"/>
@@ -1928,7 +1950,7 @@
     </row>
     <row r="52" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="80"/>
-      <c r="B52" s="52"/>
+      <c r="B52" s="54"/>
       <c r="C52" s="81"/>
       <c r="D52" s="81"/>
       <c r="E52" s="81"/>
@@ -1936,7 +1958,7 @@
     </row>
     <row r="53" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="80"/>
-      <c r="B53" s="52"/>
+      <c r="B53" s="54"/>
       <c r="C53" s="81"/>
       <c r="D53" s="81"/>
       <c r="E53" s="81"/>
@@ -1944,18 +1966,18 @@
     </row>
     <row r="54" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="80"/>
-      <c r="B54" s="52"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="81"/>
       <c r="D54" s="81"/>
       <c r="E54" s="81"/>
-      <c r="F54" s="52"/>
+      <c r="F54" s="54"/>
     </row>
     <row r="55" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="80"/>
       <c r="B55" s="81"/>
       <c r="C55" s="81"/>
       <c r="D55" s="81"/>
-      <c r="E55" s="52"/>
+      <c r="E55" s="54"/>
       <c r="F55" s="81"/>
     </row>
     <row r="56" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1963,7 +1985,7 @@
       <c r="B56" s="81"/>
       <c r="C56" s="81"/>
       <c r="D56" s="81"/>
-      <c r="E56" s="52"/>
+      <c r="E56" s="54"/>
       <c r="F56" s="81"/>
     </row>
     <row r="57" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1971,7 +1993,7 @@
       <c r="B57" s="81"/>
       <c r="C57" s="81"/>
       <c r="D57" s="81"/>
-      <c r="E57" s="52"/>
+      <c r="E57" s="54"/>
       <c r="F57" s="81"/>
     </row>
     <row r="58" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1979,7 +2001,7 @@
       <c r="B58" s="81"/>
       <c r="C58" s="81"/>
       <c r="D58" s="81"/>
-      <c r="E58" s="52"/>
+      <c r="E58" s="54"/>
       <c r="F58" s="81"/>
     </row>
     <row r="59" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1987,7 +2009,7 @@
       <c r="B59" s="81"/>
       <c r="C59" s="81"/>
       <c r="D59" s="81"/>
-      <c r="E59" s="52"/>
+      <c r="E59" s="54"/>
       <c r="F59" s="81"/>
     </row>
     <row r="60" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1995,7 +2017,7 @@
       <c r="B60" s="81"/>
       <c r="C60" s="81"/>
       <c r="D60" s="81"/>
-      <c r="E60" s="52"/>
+      <c r="E60" s="54"/>
       <c r="F60" s="81"/>
     </row>
     <row r="61" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2003,7 +2025,7 @@
       <c r="B61" s="81"/>
       <c r="C61" s="81"/>
       <c r="D61" s="81"/>
-      <c r="E61" s="52"/>
+      <c r="E61" s="54"/>
       <c r="F61" s="81"/>
     </row>
     <row r="62" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2011,7 +2033,7 @@
       <c r="B62" s="81"/>
       <c r="C62" s="81"/>
       <c r="D62" s="81"/>
-      <c r="E62" s="52"/>
+      <c r="E62" s="54"/>
       <c r="F62" s="81"/>
     </row>
     <row r="63" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2019,7 +2041,7 @@
       <c r="B63" s="81"/>
       <c r="C63" s="81"/>
       <c r="D63" s="81"/>
-      <c r="E63" s="52"/>
+      <c r="E63" s="54"/>
       <c r="F63" s="81"/>
     </row>
     <row r="64" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2027,7 +2049,7 @@
       <c r="B64" s="81"/>
       <c r="C64" s="81"/>
       <c r="D64" s="81"/>
-      <c r="E64" s="52"/>
+      <c r="E64" s="54"/>
       <c r="F64" s="81"/>
     </row>
     <row r="65" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2035,7 +2057,7 @@
       <c r="B65" s="81"/>
       <c r="C65" s="81"/>
       <c r="D65" s="81"/>
-      <c r="E65" s="52"/>
+      <c r="E65" s="54"/>
       <c r="F65" s="81"/>
     </row>
     <row r="66" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2043,7 +2065,7 @@
       <c r="B66" s="81"/>
       <c r="C66" s="81"/>
       <c r="D66" s="81"/>
-      <c r="E66" s="52"/>
+      <c r="E66" s="54"/>
       <c r="F66" s="81"/>
     </row>
     <row r="67" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2051,7 +2073,7 @@
       <c r="B67" s="81"/>
       <c r="C67" s="81"/>
       <c r="D67" s="81"/>
-      <c r="E67" s="52"/>
+      <c r="E67" s="54"/>
       <c r="F67" s="81"/>
     </row>
     <row r="68" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2059,7 +2081,7 @@
       <c r="B68" s="81"/>
       <c r="C68" s="81"/>
       <c r="D68" s="81"/>
-      <c r="E68" s="52"/>
+      <c r="E68" s="54"/>
       <c r="F68" s="81"/>
     </row>
     <row r="69" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2067,7 +2089,7 @@
       <c r="B69" s="81"/>
       <c r="C69" s="81"/>
       <c r="D69" s="81"/>
-      <c r="E69" s="52"/>
+      <c r="E69" s="54"/>
       <c r="F69" s="81"/>
     </row>
     <row r="70" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2075,7 +2097,7 @@
       <c r="B70" s="81"/>
       <c r="C70" s="81"/>
       <c r="D70" s="81"/>
-      <c r="E70" s="52"/>
+      <c r="E70" s="54"/>
       <c r="F70" s="81"/>
     </row>
     <row r="71" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2083,7 +2105,7 @@
       <c r="B71" s="81"/>
       <c r="C71" s="81"/>
       <c r="D71" s="81"/>
-      <c r="E71" s="52"/>
+      <c r="E71" s="54"/>
       <c r="F71" s="81"/>
     </row>
     <row r="72" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2091,7 +2113,7 @@
       <c r="B72" s="81"/>
       <c r="C72" s="81"/>
       <c r="D72" s="81"/>
-      <c r="E72" s="52"/>
+      <c r="E72" s="54"/>
       <c r="F72" s="81"/>
     </row>
     <row r="73" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2099,7 +2121,7 @@
       <c r="B73" s="81"/>
       <c r="C73" s="81"/>
       <c r="D73" s="81"/>
-      <c r="E73" s="52"/>
+      <c r="E73" s="54"/>
       <c r="F73" s="81"/>
     </row>
     <row r="74" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2107,7 +2129,7 @@
       <c r="B74" s="81"/>
       <c r="C74" s="81"/>
       <c r="D74" s="81"/>
-      <c r="E74" s="52"/>
+      <c r="E74" s="54"/>
       <c r="F74" s="81"/>
     </row>
     <row r="75" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2115,7 +2137,7 @@
       <c r="B75" s="81"/>
       <c r="C75" s="81"/>
       <c r="D75" s="81"/>
-      <c r="E75" s="52"/>
+      <c r="E75" s="54"/>
       <c r="F75" s="81"/>
     </row>
     <row r="76" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2123,7 +2145,7 @@
       <c r="B76" s="81"/>
       <c r="C76" s="81"/>
       <c r="D76" s="81"/>
-      <c r="E76" s="52"/>
+      <c r="E76" s="54"/>
       <c r="F76" s="81"/>
     </row>
     <row r="77" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2131,7 +2153,7 @@
       <c r="B77" s="81"/>
       <c r="C77" s="81"/>
       <c r="D77" s="81"/>
-      <c r="E77" s="52"/>
+      <c r="E77" s="54"/>
       <c r="F77" s="81"/>
     </row>
     <row r="78" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2139,7 +2161,7 @@
       <c r="B78" s="81"/>
       <c r="C78" s="81"/>
       <c r="D78" s="81"/>
-      <c r="E78" s="52"/>
+      <c r="E78" s="54"/>
       <c r="F78" s="81"/>
     </row>
     <row r="79" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2147,7 +2169,7 @@
       <c r="B79" s="81"/>
       <c r="C79" s="81"/>
       <c r="D79" s="81"/>
-      <c r="E79" s="52"/>
+      <c r="E79" s="54"/>
       <c r="F79" s="81"/>
     </row>
     <row r="80" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2155,7 +2177,7 @@
       <c r="B80" s="81"/>
       <c r="C80" s="81"/>
       <c r="D80" s="81"/>
-      <c r="E80" s="52"/>
+      <c r="E80" s="54"/>
       <c r="F80" s="81"/>
     </row>
     <row r="81" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2163,7 +2185,7 @@
       <c r="B81" s="81"/>
       <c r="C81" s="81"/>
       <c r="D81" s="81"/>
-      <c r="E81" s="52"/>
+      <c r="E81" s="54"/>
       <c r="F81" s="81"/>
     </row>
     <row r="82" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2171,7 +2193,7 @@
       <c r="B82" s="81"/>
       <c r="C82" s="81"/>
       <c r="D82" s="81"/>
-      <c r="E82" s="52"/>
+      <c r="E82" s="54"/>
       <c r="F82" s="81"/>
     </row>
     <row r="83" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2179,7 +2201,7 @@
       <c r="B83" s="81"/>
       <c r="C83" s="81"/>
       <c r="D83" s="81"/>
-      <c r="E83" s="52"/>
+      <c r="E83" s="54"/>
       <c r="F83" s="81"/>
     </row>
     <row r="84" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2187,7 +2209,7 @@
       <c r="B84" s="81"/>
       <c r="C84" s="81"/>
       <c r="D84" s="81"/>
-      <c r="E84" s="52"/>
+      <c r="E84" s="54"/>
       <c r="F84" s="81"/>
     </row>
     <row r="85" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2195,7 +2217,7 @@
       <c r="B85" s="81"/>
       <c r="C85" s="81"/>
       <c r="D85" s="81"/>
-      <c r="E85" s="52"/>
+      <c r="E85" s="54"/>
       <c r="F85" s="81"/>
     </row>
     <row r="86" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2203,7 +2225,7 @@
       <c r="B86" s="81"/>
       <c r="C86" s="81"/>
       <c r="D86" s="81"/>
-      <c r="E86" s="52"/>
+      <c r="E86" s="54"/>
       <c r="F86" s="81"/>
     </row>
     <row r="87" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2211,7 +2233,7 @@
       <c r="B87" s="81"/>
       <c r="C87" s="81"/>
       <c r="D87" s="81"/>
-      <c r="E87" s="52"/>
+      <c r="E87" s="54"/>
       <c r="F87" s="81"/>
     </row>
     <row r="88" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2219,7 +2241,7 @@
       <c r="B88" s="81"/>
       <c r="C88" s="81"/>
       <c r="D88" s="81"/>
-      <c r="E88" s="52"/>
+      <c r="E88" s="54"/>
       <c r="F88" s="81"/>
     </row>
     <row r="89" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2227,7 +2249,7 @@
       <c r="B89" s="81"/>
       <c r="C89" s="81"/>
       <c r="D89" s="81"/>
-      <c r="E89" s="52"/>
+      <c r="E89" s="54"/>
       <c r="F89" s="81"/>
     </row>
   </sheetData>

</xml_diff>